<commit_message>
changes for remote system
</commit_message>
<xml_diff>
--- a/persistance/data/Serhat_list.xlsx
+++ b/persistance/data/Serhat_list.xlsx
@@ -447,7 +447,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -475,20 +475,23 @@
           <t>B00DHHOQSA</t>
         </is>
       </c>
+      <c r="F2" t="n">
+        <v>0.3145330535152152</v>
+      </c>
       <c r="J2" t="n">
-        <v>-0.9514885495998048</v>
+        <v>28.0946659139879</v>
       </c>
       <c r="K2" t="n">
         <v>11.99</v>
       </c>
       <c r="L2" t="n">
-        <v>39.16</v>
+        <v>38.12</v>
       </c>
       <c r="M2" t="n">
-        <v>0</v>
+        <v>387</v>
       </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3">
@@ -497,20 +500,23 @@
           <t>B007TWNKHW</t>
         </is>
       </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>169.5756191487949</v>
       </c>
       <c r="K3" t="n">
-        <v>18.3</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>39.5</v>
+        <v>24.99</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4">
@@ -519,20 +525,23 @@
           <t>B07G8SMWN3</t>
         </is>
       </c>
+      <c r="F4" t="n">
+        <v>0.4717977215893304</v>
+      </c>
       <c r="J4" t="n">
-        <v>-0.9643009628744293</v>
+        <v>-97.8168688737677</v>
       </c>
       <c r="K4" t="n">
-        <v>17.16</v>
+        <v>16.98</v>
       </c>
       <c r="L4" t="n">
-        <v>49.49</v>
+        <v>35.99</v>
       </c>
       <c r="M4" t="n">
-        <v>0</v>
+        <v>768</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5">
@@ -541,17 +550,20 @@
           <t>B0060BELNA</t>
         </is>
       </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
       <c r="J5" t="n">
-        <v>-0.9573507478759606</v>
+        <v>342.0548743438145</v>
       </c>
       <c r="K5" t="n">
-        <v>13.97</v>
+        <v>16.73</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1.446</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -563,20 +575,23 @@
           <t>B07Q3W1VL6</t>
         </is>
       </c>
+      <c r="F6" t="n">
+        <v>0.3715613382899628</v>
+      </c>
       <c r="J6" t="n">
-        <v>-0.9649104338824851</v>
+        <v>-68.1639571430708</v>
       </c>
       <c r="K6" t="n">
-        <v>17.5</v>
+        <v>19.99</v>
       </c>
       <c r="L6" t="n">
         <v>53.8</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
@@ -585,20 +600,23 @@
           <t>B071GZ83PV</t>
         </is>
       </c>
+      <c r="F7" t="n">
+        <v>0.3051963893632593</v>
+      </c>
       <c r="J7" t="n">
-        <v>-0.950805534770894</v>
+        <v>241.4145356880589</v>
       </c>
       <c r="K7" t="n">
-        <v>11.79</v>
+        <v>12.51</v>
       </c>
       <c r="L7" t="n">
-        <v>41.49</v>
+        <v>40.99</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>3.586</v>
       </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
@@ -607,20 +625,23 @@
           <t>B008U4SGYA</t>
         </is>
       </c>
+      <c r="F8" t="n">
+        <v>0.3642767295597484</v>
+      </c>
       <c r="J8" t="n">
-        <v>-0.9603962435044889</v>
+        <v>-93.5356860437992</v>
       </c>
       <c r="K8" t="n">
-        <v>15.23</v>
+        <v>14.48</v>
       </c>
       <c r="L8" t="n">
-        <v>44.98</v>
+        <v>39.75</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -629,20 +650,23 @@
           <t>B0BT8KJS9H</t>
         </is>
       </c>
+      <c r="F9" t="n">
+        <v>0.3566666666666667</v>
+      </c>
       <c r="J9" t="n">
-        <v>-0.9598270635431405</v>
+        <v>91.75987803982652</v>
       </c>
       <c r="K9" t="n">
         <v>14.98</v>
       </c>
       <c r="L9" t="n">
-        <v>45.23</v>
+        <v>42</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>7.885</v>
       </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10">
@@ -651,20 +675,23 @@
           <t>B0BB51JNXR</t>
         </is>
       </c>
+      <c r="F10" t="n">
+        <v>0.3827730169193584</v>
+      </c>
       <c r="J10" t="n">
-        <v>-0.9620522161505768</v>
+        <v>-90.5026128208562</v>
       </c>
       <c r="K10" t="n">
-        <v>16</v>
+        <v>17.42</v>
       </c>
       <c r="L10" t="n">
-        <v>44.99</v>
+        <v>45.51</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>247</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -673,20 +700,23 @@
           <t>B00TWVI79Y</t>
         </is>
       </c>
+      <c r="F11" t="n">
+        <v>0.3678215472235406</v>
+      </c>
       <c r="J11" t="n">
-        <v>-0.9609931152848478</v>
+        <v>-97.05295277126103</v>
       </c>
       <c r="K11" t="n">
         <v>15.5</v>
       </c>
       <c r="L11" t="n">
-        <v>47.95</v>
+        <v>42.14</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>671</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -695,20 +725,23 @@
           <t>B07G7L2GDV</t>
         </is>
       </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
       <c r="J12" t="n">
-        <v>-0.9529264008985409</v>
+        <v>691.0690657990839</v>
       </c>
       <c r="K12" t="n">
-        <v>12.43</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>46.25</v>
+        <v>40</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
@@ -717,17 +750,20 @@
           <t>B001R91KCU</t>
         </is>
       </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
       <c r="J13" t="n">
-        <v>-0.9673682493065753</v>
+        <v>143.2663437951537</v>
       </c>
       <c r="K13" t="n">
         <v>19</v>
       </c>
       <c r="L13" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>5.311</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
@@ -739,20 +775,23 @@
           <t>B0B5XTG558</t>
         </is>
       </c>
+      <c r="F14" t="n">
+        <v>0.4862797389290477</v>
+      </c>
       <c r="J14" t="n">
-        <v>-0.990557244392396</v>
+        <v>-74.93311631577436</v>
       </c>
       <c r="K14" t="n">
-        <v>71.59</v>
+        <v>69.29000000000001</v>
       </c>
       <c r="L14" t="n">
-        <v>159</v>
+        <v>142.49</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>313</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15">
@@ -761,20 +800,23 @@
           <t>B08GPHK5SN</t>
         </is>
       </c>
+      <c r="F15" t="n">
+        <v>0.4539119417168198</v>
+      </c>
       <c r="J15" t="n">
-        <v>-0.9846093917493104</v>
+        <v>22.96479565824042</v>
       </c>
       <c r="K15" t="n">
         <v>42.99</v>
       </c>
       <c r="L15" t="n">
-        <v>109.99</v>
+        <v>94.70999999999999</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -782,9 +824,6 @@
         <is>
           <t>B08B2GFJ1C</t>
         </is>
-      </c>
-      <c r="J16" t="n">
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>